<commit_message>
code developed for well screens for Lowry project. the final .csv is missing IP-21, 36, 41, and 50. CSV should be ready to go (if we don't need to add the 4 wells listed above).
</commit_message>
<xml_diff>
--- a/L1B Water Levels.1.xlsx
+++ b/L1B Water Levels.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Shared\KGS\TRI\Projects\B031-002 - MSTJV LAFB 1B\5. Field\10. Water Levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trihydrocorp-my.sharepoint.com/personal/mvanamburg_trihydro_com/Documents/Documents/LOWRY/Lowry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B65B6C3B-F569-4201-802E-9898E382A3B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{B65B6C3B-F569-4201-802E-9898E382A3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49AC1AC7-9877-4FFB-9DD5-C78F26E21759}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{9351323E-AF21-451E-B533-C7E764CCEF36}"/>
+    <workbookView xWindow="31470" yWindow="1665" windowWidth="22950" windowHeight="12540" xr2:uid="{9351323E-AF21-451E-B533-C7E764CCEF36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -652,13 +654,14 @@
   <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="3"/>
+    <col min="3" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="12.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>